<commit_message>
Chinese version of SEM update
</commit_message>
<xml_diff>
--- a/out/fit_indices.xlsx
+++ b/out/fit_indices.xlsx
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>948.1277447807877</v>
+        <v>509.7618600982453</v>
       </c>
     </row>
     <row r="5">
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5017.519868931492</v>
+        <v>3397.25108424776</v>
       </c>
     </row>
     <row r="7">
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.8367427237632004</v>
+        <v>0.8909465299377146</v>
       </c>
     </row>
     <row r="8">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.8110365739353422</v>
+        <v>0.8499487239957362</v>
       </c>
     </row>
     <row r="9">
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.7756059315482189</v>
+        <v>0.8218141097449367</v>
       </c>
     </row>
     <row r="10">
@@ -527,7 +527,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.8110365739353421</v>
+        <v>0.8499487239957361</v>
       </c>
     </row>
     <row r="11">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.8061319844688003</v>
+        <v>0.8704990043010362</v>
       </c>
     </row>
     <row r="12">
@@ -547,7 +547,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.1298813790327612</v>
+        <v>0.08652364522839813</v>
       </c>
     </row>
     <row r="13">
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>93.528138260882</v>
+        <v>96.52039685939764</v>
       </c>
     </row>
     <row r="14">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>277.5367687117354</v>
+        <v>280.529027310251</v>
       </c>
     </row>
     <row r="15">
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>3.235930869559002</v>
+        <v>1.739801570301179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>